<commit_message>
STMT-1A -> 1. source code and excel file change as per latest format of Statement 1A 2. Download link for it added into readme.md file
</commit_message>
<xml_diff>
--- a/Stmt_1A_Json_Generator/GST_Stmt1A_Template.xlsx
+++ b/Stmt_1A_Json_Generator/GST_Stmt1A_Template.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
     <sheet name="stmt1A" sheetId="2" r:id="rId2"/>
+    <sheet name="instructions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>GSTIN</t>
   </si>
@@ -72,7 +73,70 @@
 (dd-mm-yyyy) </t>
   </si>
   <si>
-    <t>00XXXXX0000X1Z0</t>
+    <t>Type of Inward Supply</t>
+  </si>
+  <si>
+    <t>Type of Document</t>
+  </si>
+  <si>
+    <t>Port Code</t>
+  </si>
+  <si>
+    <t>Type of Outward Supply</t>
+  </si>
+  <si>
+    <t>Import of Goods/Supplies from SEZ to DTA</t>
+  </si>
+  <si>
+    <t>Import of Services/Supplies from SEZ to DTA</t>
+  </si>
+  <si>
+    <t>Inward supplies liable to reverse charge</t>
+  </si>
+  <si>
+    <t>Inward Supply from Registered Person</t>
+  </si>
+  <si>
+    <t>Inward Supplies from ISD</t>
+  </si>
+  <si>
+    <t>Invoice/Bill of Entry</t>
+  </si>
+  <si>
+    <t>Debit Note</t>
+  </si>
+  <si>
+    <t>Credit Note</t>
+  </si>
+  <si>
+    <t>B2B</t>
+  </si>
+  <si>
+    <t>B2C-Large</t>
+  </si>
+  <si>
+    <t>B2C-Small</t>
+  </si>
+  <si>
+    <t>In case of "B2C-Small" Outward Supply</t>
+  </si>
+  <si>
+    <t>Document No - B2COTH</t>
+  </si>
+  <si>
+    <t>Document Date - 01-07-2017</t>
+  </si>
+  <si>
+    <t>Cell values for reference</t>
+  </si>
+  <si>
+    <t>In case of Import of Goods/Service or RCM purchase from Unregistered Person</t>
+  </si>
+  <si>
+    <t>GSTIN of refund claimer should be entered</t>
+  </si>
+  <si>
+    <t>24XXXXX0000X1ZX</t>
   </si>
 </sst>
 </file>
@@ -104,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -127,11 +191,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -141,7 +242,22 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,13 +566,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -464,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -472,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>12017</v>
+        <v>72017</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -480,7 +596,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>12017</v>
+        <v>72017</v>
       </c>
     </row>
   </sheetData>
@@ -490,152 +606,320 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12" style="4" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-    </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
       <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="3"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="3"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B1:E1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>